<commit_message>
Profit of generators and wind in step 3
</commit_message>
<xml_diff>
--- a/results_step3_nodal.xlsx
+++ b/results_step3_nodal.xlsx
@@ -21,6 +21,8 @@
     <sheet name="Nodal_Generation" r:id="rId9" sheetId="6"/>
     <sheet name="Nodal_Demand" r:id="rId10" sheetId="7"/>
     <sheet name="Nodal_Wind" r:id="rId11" sheetId="8"/>
+    <sheet name="Profit_gen" r:id="rId12" sheetId="9"/>
+    <sheet name="Profit_wind" r:id="rId13" sheetId="10"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -2367,6 +2369,519 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+  <dimension ref="A1:F25"/>
+  <sheetViews>
+    <sheetView tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <v>0.0</v>
+      </c>
+      <c r="B2">
+        <v>1764.1645106693788</v>
+      </c>
+      <c r="C2">
+        <v>24.56961514124597</v>
+      </c>
+      <c r="D2">
+        <v>59.71755929916871</v>
+      </c>
+      <c r="E2">
+        <v>127.08651232915894</v>
+      </c>
+      <c r="F2">
+        <v>66.59913855616138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>0.0</v>
+      </c>
+      <c r="B3">
+        <v>0.0</v>
+      </c>
+      <c r="C3">
+        <v>57.06788892703634</v>
+      </c>
+      <c r="D3">
+        <v>106.29970933910111</v>
+      </c>
+      <c r="E3">
+        <v>270.8297164496531</v>
+      </c>
+      <c r="F3">
+        <v>166.36487431802777</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>0.0</v>
+      </c>
+      <c r="B4">
+        <v>273.71214120050894</v>
+      </c>
+      <c r="C4">
+        <v>67.52417745099999</v>
+      </c>
+      <c r="D4">
+        <v>101.1217010128746</v>
+      </c>
+      <c r="E4">
+        <v>303.11297057659317</v>
+      </c>
+      <c r="F4">
+        <v>150.6157284648102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>603.7008952602121</v>
+      </c>
+      <c r="B5">
+        <v>565.4896077852261</v>
+      </c>
+      <c r="C5">
+        <v>81.3636065392419</v>
+      </c>
+      <c r="D5">
+        <v>132.78213915675806</v>
+      </c>
+      <c r="E5">
+        <v>364.4929144614483</v>
+      </c>
+      <c r="F5">
+        <v>229.82430895691834</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>35.152804974970806</v>
+      </c>
+      <c r="B6">
+        <v>721.4715597694662</v>
+      </c>
+      <c r="C6">
+        <v>82.88974384899849</v>
+      </c>
+      <c r="D6">
+        <v>163.64768352234205</v>
+      </c>
+      <c r="E6">
+        <v>370.8949244992298</v>
+      </c>
+      <c r="F6">
+        <v>239.8082906082434</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>553.1258632030689</v>
+      </c>
+      <c r="B7">
+        <v>509.6813907170629</v>
+      </c>
+      <c r="C7">
+        <v>68.55834072377009</v>
+      </c>
+      <c r="D7">
+        <v>88.5196783832</v>
+      </c>
+      <c r="E7">
+        <v>315.7506225320713</v>
+      </c>
+      <c r="F7">
+        <v>127.3598853348</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>736.7149796399449</v>
+      </c>
+      <c r="B8">
+        <v>850.8752272215812</v>
+      </c>
+      <c r="C8">
+        <v>72.90980180423728</v>
+      </c>
+      <c r="D8">
+        <v>158.32526935747305</v>
+      </c>
+      <c r="E8">
+        <v>393.63137894375956</v>
+      </c>
+      <c r="F8">
+        <v>228.09853001232665</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <v>2324.686195821684</v>
+      </c>
+      <c r="B9">
+        <v>2525.5438299487514</v>
+      </c>
+      <c r="C9">
+        <v>79.18315579323271</v>
+      </c>
+      <c r="D9">
+        <v>169.67829055176574</v>
+      </c>
+      <c r="E9">
+        <v>404.45377960018504</v>
+      </c>
+      <c r="F9">
+        <v>244.8346014185639</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10">
+        <v>2261.688907290222</v>
+      </c>
+      <c r="B10">
+        <v>2369.046941785402</v>
+      </c>
+      <c r="C10">
+        <v>88.02688520599075</v>
+      </c>
+      <c r="D10">
+        <v>184.0959060237658</v>
+      </c>
+      <c r="E10">
+        <v>384.7155687432974</v>
+      </c>
+      <c r="F10">
+        <v>248.18868668679198</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11">
+        <v>2188.8049364883227</v>
+      </c>
+      <c r="B11">
+        <v>1690.5447426749615</v>
+      </c>
+      <c r="C11">
+        <v>87.6507466104</v>
+      </c>
+      <c r="D11">
+        <v>174.92877461546666</v>
+      </c>
+      <c r="E11">
+        <v>393.617401982</v>
+      </c>
+      <c r="F11">
+        <v>221.5342059084</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12">
+        <v>1027.9318716596445</v>
+      </c>
+      <c r="B12">
+        <v>507.42856893374227</v>
+      </c>
+      <c r="C12">
+        <v>80.51940419542758</v>
+      </c>
+      <c r="D12">
+        <v>184.78093259913416</v>
+      </c>
+      <c r="E12">
+        <v>425.4533482773728</v>
+      </c>
+      <c r="F12">
+        <v>218.18539890617083</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13">
+        <v>3068.7019946498112</v>
+      </c>
+      <c r="B13">
+        <v>880.9958888170329</v>
+      </c>
+      <c r="C13">
+        <v>61.38658736221934</v>
+      </c>
+      <c r="D13">
+        <v>166.8825564239656</v>
+      </c>
+      <c r="E13">
+        <v>369.83850717187084</v>
+      </c>
+      <c r="F13">
+        <v>232.74593811375487</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14">
+        <v>3535.4837346624263</v>
+      </c>
+      <c r="B14">
+        <v>670.2285187503554</v>
+      </c>
+      <c r="C14">
+        <v>62.00012938403007</v>
+      </c>
+      <c r="D14">
+        <v>83.78086662999999</v>
+      </c>
+      <c r="E14">
+        <v>354.6703556478489</v>
+      </c>
+      <c r="F14">
+        <v>122.00111991809999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15">
+        <v>2413.1983214506836</v>
+      </c>
+      <c r="B15">
+        <v>536.6913256903616</v>
+      </c>
+      <c r="C15">
+        <v>72.3148889124</v>
+      </c>
+      <c r="D15">
+        <v>142.5762548144</v>
+      </c>
+      <c r="E15">
+        <v>393.19459055799996</v>
+      </c>
+      <c r="F15">
+        <v>189.6923788584</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16">
+        <v>1697.5274818980781</v>
+      </c>
+      <c r="B16">
+        <v>924.4218857102076</v>
+      </c>
+      <c r="C16">
+        <v>71.699423992</v>
+      </c>
+      <c r="D16">
+        <v>139.8161149352</v>
+      </c>
+      <c r="E16">
+        <v>391.75955052</v>
+      </c>
+      <c r="F16">
+        <v>143.5620925464</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17">
+        <v>2581.2339400956103</v>
+      </c>
+      <c r="B17">
+        <v>2042.212990968979</v>
+      </c>
+      <c r="C17">
+        <v>55.55708445063268</v>
+      </c>
+      <c r="D17">
+        <v>79.5734814586</v>
+      </c>
+      <c r="E17">
+        <v>302.3876695817348</v>
+      </c>
+      <c r="F17">
+        <v>89.45287411289999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18">
+        <v>1207.8420700213378</v>
+      </c>
+      <c r="B18">
+        <v>1729.3274248472937</v>
+      </c>
+      <c r="C18">
+        <v>69.5631720453778</v>
+      </c>
+      <c r="D18">
+        <v>143.341538527427</v>
+      </c>
+      <c r="E18">
+        <v>371.96259277632697</v>
+      </c>
+      <c r="F18">
+        <v>141.56280425045657</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19">
+        <v>497.34267158347666</v>
+      </c>
+      <c r="B19">
+        <v>716.2908989043865</v>
+      </c>
+      <c r="C19">
+        <v>70.43685818952872</v>
+      </c>
+      <c r="D19">
+        <v>145.13721899865888</v>
+      </c>
+      <c r="E19">
+        <v>373.85750972217227</v>
+      </c>
+      <c r="F19">
+        <v>132.96338508450998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20">
+        <v>2785.5432192414805</v>
+      </c>
+      <c r="B20">
+        <v>3122.1419819364464</v>
+      </c>
+      <c r="C20">
+        <v>47.35125585571851</v>
+      </c>
+      <c r="D20">
+        <v>158.50941891914272</v>
+      </c>
+      <c r="E20">
+        <v>320.1337230693778</v>
+      </c>
+      <c r="F20">
+        <v>168.05367503624888</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21">
+        <v>2536.89164316</v>
+      </c>
+      <c r="B21">
+        <v>2948.0605530884995</v>
+      </c>
+      <c r="C21">
+        <v>60.05645001720001</v>
+      </c>
+      <c r="D21">
+        <v>153.9075104196</v>
+      </c>
+      <c r="E21">
+        <v>368.43240295399994</v>
+      </c>
+      <c r="F21">
+        <v>197.1204255432</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22">
+        <v>999.2420089324289</v>
+      </c>
+      <c r="B22">
+        <v>2695.88155307651</v>
+      </c>
+      <c r="C22">
+        <v>69.81371788497442</v>
+      </c>
+      <c r="D22">
+        <v>146.1744108914071</v>
+      </c>
+      <c r="E22">
+        <v>411.3536329917461</v>
+      </c>
+      <c r="F22">
+        <v>203.44053090802623</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23">
+        <v>2059.5467275024857</v>
+      </c>
+      <c r="B23">
+        <v>939.0368205995104</v>
+      </c>
+      <c r="C23">
+        <v>85.8990962316</v>
+      </c>
+      <c r="D23">
+        <v>152.26321811946667</v>
+      </c>
+      <c r="E23">
+        <v>399.54399073599996</v>
+      </c>
+      <c r="F23">
+        <v>188.83870320920002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24">
+        <v>2025.5156256020166</v>
+      </c>
+      <c r="B24">
+        <v>2013.2748130493144</v>
+      </c>
+      <c r="C24">
+        <v>83.25148657916792</v>
+      </c>
+      <c r="D24">
+        <v>150.6486088693005</v>
+      </c>
+      <c r="E24">
+        <v>409.0565846319876</v>
+      </c>
+      <c r="F24">
+        <v>95.22081841556857</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25">
+        <v>592.6046382804761</v>
+      </c>
+      <c r="B25">
+        <v>824.3680575480814</v>
+      </c>
+      <c r="C25">
+        <v>83.51396095058809</v>
+      </c>
+      <c r="D25">
+        <v>127.20775752661977</v>
+      </c>
+      <c r="E25">
+        <v>408.45884784385777</v>
+      </c>
+      <c r="F25">
+        <v>47.524835987033</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
   <dimension ref="A1:X25"/>
@@ -12631,4 +13146,967 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+  <dimension ref="A1:L25"/>
+  <sheetViews>
+    <sheetView tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2">
+        <v>0.0</v>
+      </c>
+      <c r="B2">
+        <v>0.0</v>
+      </c>
+      <c r="C2">
+        <v>0.0</v>
+      </c>
+      <c r="D2">
+        <v>0.0</v>
+      </c>
+      <c r="E2">
+        <v>0.0</v>
+      </c>
+      <c r="F2">
+        <v>0.0</v>
+      </c>
+      <c r="G2">
+        <v>0.0</v>
+      </c>
+      <c r="H2">
+        <v>0.0</v>
+      </c>
+      <c r="I2">
+        <v>316.64547677261635</v>
+      </c>
+      <c r="J2">
+        <v>0.0</v>
+      </c>
+      <c r="K2">
+        <v>107.99823960880212</v>
+      </c>
+      <c r="L2">
+        <v>-0.8647432762836615</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3">
+        <v>0.0</v>
+      </c>
+      <c r="B3">
+        <v>0.0</v>
+      </c>
+      <c r="C3">
+        <v>0.0</v>
+      </c>
+      <c r="D3">
+        <v>0.0</v>
+      </c>
+      <c r="E3">
+        <v>0.0</v>
+      </c>
+      <c r="F3">
+        <v>28.030733679950345</v>
+      </c>
+      <c r="G3">
+        <v>0.0</v>
+      </c>
+      <c r="H3">
+        <v>1592.0</v>
+      </c>
+      <c r="I3">
+        <v>1751.318313113808</v>
+      </c>
+      <c r="J3">
+        <v>0.0</v>
+      </c>
+      <c r="K3">
+        <v>0.0</v>
+      </c>
+      <c r="L3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4">
+        <v>0.0</v>
+      </c>
+      <c r="B4">
+        <v>0.0</v>
+      </c>
+      <c r="C4">
+        <v>0.0</v>
+      </c>
+      <c r="D4">
+        <v>0.0</v>
+      </c>
+      <c r="E4">
+        <v>0.0</v>
+      </c>
+      <c r="F4">
+        <v>0.0</v>
+      </c>
+      <c r="G4">
+        <v>0.0</v>
+      </c>
+      <c r="H4">
+        <v>788.0</v>
+      </c>
+      <c r="I4">
+        <v>813.0847457627124</v>
+      </c>
+      <c r="J4">
+        <v>0.0</v>
+      </c>
+      <c r="K4">
+        <v>0.0</v>
+      </c>
+      <c r="L4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5">
+        <v>0.0</v>
+      </c>
+      <c r="B5">
+        <v>0.0</v>
+      </c>
+      <c r="C5">
+        <v>0.0</v>
+      </c>
+      <c r="D5">
+        <v>0.0</v>
+      </c>
+      <c r="E5">
+        <v>0.0</v>
+      </c>
+      <c r="F5">
+        <v>0.0</v>
+      </c>
+      <c r="G5">
+        <v>0.0</v>
+      </c>
+      <c r="H5">
+        <v>1592.0</v>
+      </c>
+      <c r="I5">
+        <v>1785.62095531587</v>
+      </c>
+      <c r="J5">
+        <v>0.0</v>
+      </c>
+      <c r="K5">
+        <v>114.70000000000027</v>
+      </c>
+      <c r="L5">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6">
+        <v>0.0</v>
+      </c>
+      <c r="B6">
+        <v>0.0</v>
+      </c>
+      <c r="C6">
+        <v>0.0</v>
+      </c>
+      <c r="D6">
+        <v>0.0</v>
+      </c>
+      <c r="E6">
+        <v>0.0</v>
+      </c>
+      <c r="F6">
+        <v>0.0</v>
+      </c>
+      <c r="G6">
+        <v>0.0</v>
+      </c>
+      <c r="H6">
+        <v>1592.0</v>
+      </c>
+      <c r="I6">
+        <v>1771.9383667180268</v>
+      </c>
+      <c r="J6">
+        <v>0.0</v>
+      </c>
+      <c r="K6">
+        <v>0.0</v>
+      </c>
+      <c r="L6">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7">
+        <v>0.0</v>
+      </c>
+      <c r="B7">
+        <v>0.0</v>
+      </c>
+      <c r="C7">
+        <v>0.0</v>
+      </c>
+      <c r="D7">
+        <v>0.0</v>
+      </c>
+      <c r="E7">
+        <v>0.0</v>
+      </c>
+      <c r="F7">
+        <v>0.0</v>
+      </c>
+      <c r="G7">
+        <v>0.0</v>
+      </c>
+      <c r="H7">
+        <v>106.22739018087941</v>
+      </c>
+      <c r="I7">
+        <v>0.0</v>
+      </c>
+      <c r="J7">
+        <v>0.0</v>
+      </c>
+      <c r="K7">
+        <v>0.0</v>
+      </c>
+      <c r="L7">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8">
+        <v>0.0</v>
+      </c>
+      <c r="B8">
+        <v>0.0</v>
+      </c>
+      <c r="C8">
+        <v>0.0</v>
+      </c>
+      <c r="D8">
+        <v>0.0</v>
+      </c>
+      <c r="E8">
+        <v>0.0</v>
+      </c>
+      <c r="F8">
+        <v>0.0</v>
+      </c>
+      <c r="G8">
+        <v>0.0</v>
+      </c>
+      <c r="H8">
+        <v>1592.0</v>
+      </c>
+      <c r="I8">
+        <v>1771.9383667180277</v>
+      </c>
+      <c r="J8">
+        <v>0.0</v>
+      </c>
+      <c r="K8">
+        <v>0.0</v>
+      </c>
+      <c r="L8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9">
+        <v>0.0</v>
+      </c>
+      <c r="B9">
+        <v>0.0</v>
+      </c>
+      <c r="C9">
+        <v>0.0</v>
+      </c>
+      <c r="D9">
+        <v>0.0</v>
+      </c>
+      <c r="E9">
+        <v>0.0</v>
+      </c>
+      <c r="F9">
+        <v>0.0</v>
+      </c>
+      <c r="G9">
+        <v>0.0</v>
+      </c>
+      <c r="H9">
+        <v>1592.0</v>
+      </c>
+      <c r="I9">
+        <v>1785.62095531587</v>
+      </c>
+      <c r="J9">
+        <v>0.0</v>
+      </c>
+      <c r="K9">
+        <v>114.70000000000027</v>
+      </c>
+      <c r="L9">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10">
+        <v>0.0</v>
+      </c>
+      <c r="B10">
+        <v>0.0</v>
+      </c>
+      <c r="C10">
+        <v>0.0</v>
+      </c>
+      <c r="D10">
+        <v>0.0</v>
+      </c>
+      <c r="E10">
+        <v>0.0</v>
+      </c>
+      <c r="F10">
+        <v>0.0</v>
+      </c>
+      <c r="G10">
+        <v>0.0</v>
+      </c>
+      <c r="H10">
+        <v>1592.0</v>
+      </c>
+      <c r="I10">
+        <v>1785.620955315871</v>
+      </c>
+      <c r="J10">
+        <v>0.0</v>
+      </c>
+      <c r="K10">
+        <v>114.70000000000027</v>
+      </c>
+      <c r="L10">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11">
+        <v>0.0</v>
+      </c>
+      <c r="B11">
+        <v>0.0</v>
+      </c>
+      <c r="C11">
+        <v>0.0</v>
+      </c>
+      <c r="D11">
+        <v>0.0</v>
+      </c>
+      <c r="E11">
+        <v>0.0</v>
+      </c>
+      <c r="F11">
+        <v>55.482622838555244</v>
+      </c>
+      <c r="G11">
+        <v>0.0</v>
+      </c>
+      <c r="H11">
+        <v>1592.0</v>
+      </c>
+      <c r="I11">
+        <v>1742.6666666666665</v>
+      </c>
+      <c r="J11">
+        <v>0.0</v>
+      </c>
+      <c r="K11">
+        <v>114.70000000000027</v>
+      </c>
+      <c r="L11">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12">
+        <v>0.0</v>
+      </c>
+      <c r="B12">
+        <v>0.0</v>
+      </c>
+      <c r="C12">
+        <v>0.0</v>
+      </c>
+      <c r="D12">
+        <v>0.0</v>
+      </c>
+      <c r="E12">
+        <v>0.0</v>
+      </c>
+      <c r="F12">
+        <v>0.0</v>
+      </c>
+      <c r="G12">
+        <v>0.0</v>
+      </c>
+      <c r="H12">
+        <v>1592.0</v>
+      </c>
+      <c r="I12">
+        <v>1759.1217967590987</v>
+      </c>
+      <c r="J12">
+        <v>0.0</v>
+      </c>
+      <c r="K12">
+        <v>10.907739788405252</v>
+      </c>
+      <c r="L12">
+        <v>-15.565331459197523</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13">
+        <v>0.0</v>
+      </c>
+      <c r="B13">
+        <v>0.0</v>
+      </c>
+      <c r="C13">
+        <v>0.0</v>
+      </c>
+      <c r="D13">
+        <v>0.0</v>
+      </c>
+      <c r="E13">
+        <v>0.0</v>
+      </c>
+      <c r="F13">
+        <v>0.0</v>
+      </c>
+      <c r="G13">
+        <v>0.0</v>
+      </c>
+      <c r="H13">
+        <v>1592.0</v>
+      </c>
+      <c r="I13">
+        <v>1869.1182795698933</v>
+      </c>
+      <c r="J13">
+        <v>0.0</v>
+      </c>
+      <c r="K13">
+        <v>218.49226021159575</v>
+      </c>
+      <c r="L13">
+        <v>95.92062968752907</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14">
+        <v>272.30120547945353</v>
+      </c>
+      <c r="B14">
+        <v>371.1104986301377</v>
+      </c>
+      <c r="C14">
+        <v>0.0</v>
+      </c>
+      <c r="D14">
+        <v>0.0</v>
+      </c>
+      <c r="E14">
+        <v>0.0</v>
+      </c>
+      <c r="F14">
+        <v>406.73656164383374</v>
+      </c>
+      <c r="G14">
+        <v>0.0</v>
+      </c>
+      <c r="H14">
+        <v>222.6712328767112</v>
+      </c>
+      <c r="I14">
+        <v>0.0</v>
+      </c>
+      <c r="J14">
+        <v>0.0</v>
+      </c>
+      <c r="K14">
+        <v>114.70000000000027</v>
+      </c>
+      <c r="L14">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15">
+        <v>0.0</v>
+      </c>
+      <c r="B15">
+        <v>-74.03806594040384</v>
+      </c>
+      <c r="C15">
+        <v>0.0</v>
+      </c>
+      <c r="D15">
+        <v>0.0</v>
+      </c>
+      <c r="E15">
+        <v>0.0</v>
+      </c>
+      <c r="F15">
+        <v>59.86282990475593</v>
+      </c>
+      <c r="G15">
+        <v>0.0</v>
+      </c>
+      <c r="H15">
+        <v>1592.0</v>
+      </c>
+      <c r="I15">
+        <v>1742.6666666666665</v>
+      </c>
+      <c r="J15">
+        <v>0.0</v>
+      </c>
+      <c r="K15">
+        <v>123.77189552377104</v>
+      </c>
+      <c r="L15">
+        <v>10.242462688127944</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16">
+        <v>0.0</v>
+      </c>
+      <c r="B16">
+        <v>0.0</v>
+      </c>
+      <c r="C16">
+        <v>0.0</v>
+      </c>
+      <c r="D16">
+        <v>0.0</v>
+      </c>
+      <c r="E16">
+        <v>0.0</v>
+      </c>
+      <c r="F16">
+        <v>55.482622838555244</v>
+      </c>
+      <c r="G16">
+        <v>0.0</v>
+      </c>
+      <c r="H16">
+        <v>1592.0</v>
+      </c>
+      <c r="I16">
+        <v>1742.6666666666665</v>
+      </c>
+      <c r="J16">
+        <v>0.0</v>
+      </c>
+      <c r="K16">
+        <v>112.94305027677683</v>
+      </c>
+      <c r="L16">
+        <v>-0.6234337727566981</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17">
+        <v>0.0</v>
+      </c>
+      <c r="B17">
+        <v>0.0</v>
+      </c>
+      <c r="C17">
+        <v>0.0</v>
+      </c>
+      <c r="D17">
+        <v>0.0</v>
+      </c>
+      <c r="E17">
+        <v>0.0</v>
+      </c>
+      <c r="F17">
+        <v>0.0</v>
+      </c>
+      <c r="G17">
+        <v>0.0</v>
+      </c>
+      <c r="H17">
+        <v>79.87074829931998</v>
+      </c>
+      <c r="I17">
+        <v>0.0</v>
+      </c>
+      <c r="J17">
+        <v>0.0</v>
+      </c>
+      <c r="K17">
+        <v>117.16817359243396</v>
+      </c>
+      <c r="L17">
+        <v>2.276778293979987</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18">
+        <v>0.0</v>
+      </c>
+      <c r="B18">
+        <v>0.0</v>
+      </c>
+      <c r="C18">
+        <v>0.0</v>
+      </c>
+      <c r="D18">
+        <v>0.0</v>
+      </c>
+      <c r="E18">
+        <v>0.0</v>
+      </c>
+      <c r="F18">
+        <v>77.94232397148016</v>
+      </c>
+      <c r="G18">
+        <v>20.213731019632633</v>
+      </c>
+      <c r="H18">
+        <v>1592.0</v>
+      </c>
+      <c r="I18">
+        <v>1725.2785109508532</v>
+      </c>
+      <c r="J18">
+        <v>0.0</v>
+      </c>
+      <c r="K18">
+        <v>112.23182640756659</v>
+      </c>
+      <c r="L18">
+        <v>-0.3659342224186162</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19">
+        <v>0.0</v>
+      </c>
+      <c r="B19">
+        <v>0.0</v>
+      </c>
+      <c r="C19">
+        <v>0.0</v>
+      </c>
+      <c r="D19">
+        <v>0.0</v>
+      </c>
+      <c r="E19">
+        <v>0.0</v>
+      </c>
+      <c r="F19">
+        <v>29.620238826888453</v>
+      </c>
+      <c r="G19">
+        <v>0.0</v>
+      </c>
+      <c r="H19">
+        <v>1592.0</v>
+      </c>
+      <c r="I19">
+        <v>1750.4304073585681</v>
+      </c>
+      <c r="J19">
+        <v>0.0</v>
+      </c>
+      <c r="K19">
+        <v>2.3587084520722783</v>
+      </c>
+      <c r="L19">
+        <v>-30.84907953626623</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20">
+        <v>0.0</v>
+      </c>
+      <c r="B20">
+        <v>0.0</v>
+      </c>
+      <c r="C20">
+        <v>0.0</v>
+      </c>
+      <c r="D20">
+        <v>0.0</v>
+      </c>
+      <c r="E20">
+        <v>0.0</v>
+      </c>
+      <c r="F20">
+        <v>0.0</v>
+      </c>
+      <c r="G20">
+        <v>0.0</v>
+      </c>
+      <c r="H20">
+        <v>1592.0</v>
+      </c>
+      <c r="I20">
+        <v>1858.8938271604939</v>
+      </c>
+      <c r="J20">
+        <v>0.0</v>
+      </c>
+      <c r="K20">
+        <v>227.04129154792827</v>
+      </c>
+      <c r="L20">
+        <v>117.82298267014585</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21">
+        <v>0.0</v>
+      </c>
+      <c r="B21">
+        <v>0.0</v>
+      </c>
+      <c r="C21">
+        <v>0.0</v>
+      </c>
+      <c r="D21">
+        <v>0.0</v>
+      </c>
+      <c r="E21">
+        <v>0.0</v>
+      </c>
+      <c r="F21">
+        <v>0.0</v>
+      </c>
+      <c r="G21">
+        <v>0.0</v>
+      </c>
+      <c r="H21">
+        <v>1592.0</v>
+      </c>
+      <c r="I21">
+        <v>1820.0</v>
+      </c>
+      <c r="J21">
+        <v>0.0</v>
+      </c>
+      <c r="K21">
+        <v>114.70000000000027</v>
+      </c>
+      <c r="L21">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22">
+        <v>0.0</v>
+      </c>
+      <c r="B22">
+        <v>0.0</v>
+      </c>
+      <c r="C22">
+        <v>0.0</v>
+      </c>
+      <c r="D22">
+        <v>0.0</v>
+      </c>
+      <c r="E22">
+        <v>0.0</v>
+      </c>
+      <c r="F22">
+        <v>0.0</v>
+      </c>
+      <c r="G22">
+        <v>0.0</v>
+      </c>
+      <c r="H22">
+        <v>1592.0</v>
+      </c>
+      <c r="I22">
+        <v>1802.4209553158707</v>
+      </c>
+      <c r="J22">
+        <v>0.0</v>
+      </c>
+      <c r="K22">
+        <v>114.70000000000027</v>
+      </c>
+      <c r="L22">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23">
+        <v>0.0</v>
+      </c>
+      <c r="B23">
+        <v>0.0</v>
+      </c>
+      <c r="C23">
+        <v>0.0</v>
+      </c>
+      <c r="D23">
+        <v>0.0</v>
+      </c>
+      <c r="E23">
+        <v>0.0</v>
+      </c>
+      <c r="F23">
+        <v>58.39171171171142</v>
+      </c>
+      <c r="G23">
+        <v>0.0</v>
+      </c>
+      <c r="H23">
+        <v>1592.0</v>
+      </c>
+      <c r="I23">
+        <v>1742.6666666666665</v>
+      </c>
+      <c r="J23">
+        <v>0.0</v>
+      </c>
+      <c r="K23">
+        <v>114.70000000000027</v>
+      </c>
+      <c r="L23">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24">
+        <v>0.0</v>
+      </c>
+      <c r="B24">
+        <v>0.0</v>
+      </c>
+      <c r="C24">
+        <v>0.0</v>
+      </c>
+      <c r="D24">
+        <v>0.0</v>
+      </c>
+      <c r="E24">
+        <v>0.0</v>
+      </c>
+      <c r="F24">
+        <v>0.0</v>
+      </c>
+      <c r="G24">
+        <v>0.0</v>
+      </c>
+      <c r="H24">
+        <v>1592.0</v>
+      </c>
+      <c r="I24">
+        <v>1785.6209553158715</v>
+      </c>
+      <c r="J24">
+        <v>0.0</v>
+      </c>
+      <c r="K24">
+        <v>114.70000000000027</v>
+      </c>
+      <c r="L24">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25">
+        <v>0.0</v>
+      </c>
+      <c r="B25">
+        <v>0.0</v>
+      </c>
+      <c r="C25">
+        <v>0.0</v>
+      </c>
+      <c r="D25">
+        <v>0.0</v>
+      </c>
+      <c r="E25">
+        <v>0.0</v>
+      </c>
+      <c r="F25">
+        <v>0.0</v>
+      </c>
+      <c r="G25">
+        <v>0.0</v>
+      </c>
+      <c r="H25">
+        <v>1592.0</v>
+      </c>
+      <c r="I25">
+        <v>1766.9764252035998</v>
+      </c>
+      <c r="J25">
+        <v>0.0</v>
+      </c>
+      <c r="K25">
+        <v>0.0</v>
+      </c>
+      <c r="L25">
+        <v>0.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>